<commit_message>
Coteja Principal + Integrantes Ok
</commit_message>
<xml_diff>
--- a/uploads/00 BHA-BPRM_Base Registro Nacional_stage_upload_50_casos.xlsx
+++ b/uploads/00 BHA-BPRM_Base Registro Nacional_stage_upload_50_casos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3719" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3720" uniqueCount="1084">
   <si>
     <t>2021-09-15</t>
   </si>
@@ -3287,6 +3287,9 @@
   </si>
   <si>
     <t>Observaciones</t>
+  </si>
+  <si>
+    <t>010141618</t>
   </si>
 </sst>
 </file>
@@ -3371,7 +3374,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3380,6 +3383,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Estilo 1" xfId="1"/>
@@ -4358,8 +4362,8 @@
       <c r="U2" t="s">
         <v>13</v>
       </c>
-      <c r="W2">
-        <v>10141618</v>
+      <c r="W2" s="4" t="s">
+        <v>1083</v>
       </c>
       <c r="X2" t="s">
         <v>14</v>

</xml_diff>